<commit_message>
Added header, total price and logo on pdf.
</commit_message>
<xml_diff>
--- a/invoices/10001-2023.1.18.xlsx
+++ b/invoices/10001-2023.1.18.xlsx
@@ -64,7 +64,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -204,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -242,20 +242,17 @@
     <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,15 +562,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="17" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="17" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="17" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="14" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="15" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="28.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -591,7 +588,7 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="30" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33" customFormat="1" s="1">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -609,7 +606,7 @@
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="30" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33" customFormat="1" s="1">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
@@ -627,60 +624,60 @@
       </c>
       <c r="F3" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A4" s="13"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A5" s="13"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A6" s="13"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A7" s="13"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A8" s="13"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A9" s="13"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A10" s="13"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="12"/>
     </row>
   </sheetData>

</xml_diff>